<commit_message>
Insercao de estrategias em partes interessadas. (#176)
</commit_message>
<xml_diff>
--- a/docs/documentos/partes interessadas.xlsx
+++ b/docs/documentos/partes interessadas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alcid\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF9975D-9D3B-4D14-9DB7-3B8223D4E85E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F43C66-2DA1-4B93-951D-2E5D24F602CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="109">
   <si>
     <t>Impacto</t>
   </si>
@@ -275,9 +275,6 @@
     <t>Desenvolvedor</t>
   </si>
   <si>
-    <t>85 99103-6233</t>
-  </si>
-  <si>
     <t>marcelo.fernandes@ifrn.edu.br</t>
   </si>
   <si>
@@ -291,45 +288,15 @@
     <t>IFRN</t>
   </si>
   <si>
-    <t>Cliente</t>
-  </si>
-  <si>
-    <t>Não informado</t>
-  </si>
-  <si>
-    <t>Aluno - Campus Natal Central</t>
-  </si>
-  <si>
-    <t>Gerente da equipe de desenvolvimento</t>
-  </si>
-  <si>
     <t>Instituto Federal do Rio Grande do Norte - Campus Natal Central</t>
   </si>
   <si>
-    <t>Prover os resultados desejados pelos clientes, entregando software de qualidade</t>
-  </si>
-  <si>
     <t>Realizar estudos através do sistema por meio de um banco de questões e responder avaliações passadas pelos professores</t>
   </si>
   <si>
-    <t>Professor do órgão onde o sistema será implantado</t>
-  </si>
-  <si>
-    <t>Órgão para implantanção inicial do sistema</t>
-  </si>
-  <si>
-    <t>Estudantes do órgão onde o sistema será implantado</t>
-  </si>
-  <si>
     <t>Aplicar o sistema em suas turmas para que seus alunos tanto estudem os conteúdos de suas disciplinas lecionadas quanto realizem suas avaliações e questões próprias elaboradas</t>
   </si>
   <si>
-    <t>Possuir um software acadêmico que possa ser aplicado no campus para permitir a aplicação e realização de atividades avaliativas por meio de um banco de questões</t>
-  </si>
-  <si>
-    <t>Fornecer ambiente virtual institucional para implantação da plataforma</t>
-  </si>
-  <si>
     <t>Desenvolver e refatorar códigos no front-end da aplicação</t>
   </si>
   <si>
@@ -339,19 +306,99 @@
     <t>Desenvolver a infraestrutura da aplicação</t>
   </si>
   <si>
-    <t>Utilizar a plataforma em sala de aula e prover feedbacks detalhados de como ela pode ser melhorada</t>
-  </si>
-  <si>
     <t>Responder questões e avaliações passadas por seus professores, além de prover feedbacks construtivos de como a aplicação pode ser melhorada</t>
   </si>
   <si>
-    <t>• Apresentar constantemente os protótipos construídos;
-• Manter contato frequente sobre o andamento do projeto;
-• Perguntar como o sistema deve ser para ter utilidade e quais funcionalidades ele deve possuir para que seu uso em sala de aula ocorra da melhor forma possível.</t>
-  </si>
-  <si>
-    <t>• Demonstrar esforço constante sob o software ofertado para a instituição, a fim de melhor atendê-la com qualidade e no menor tempo possível;
-• Oferecer disponibilidade para eventuais questionamentos e/ou reuniões.</t>
+    <t>84 99103-6233</t>
+  </si>
+  <si>
+    <t>Cliente e Patrocinador</t>
+  </si>
+  <si>
+    <t>Atual gerente da equipe de desenvolvimento</t>
+  </si>
+  <si>
+    <t>• Prover os resultados desejados pelos clientes, entregando software de qualidade;
+• Trabalhar e ampliar conhecimentos de backend e Django Rest;
+• Melhorar habilidades comunicativas por meio de trabalho em equipe.</t>
+  </si>
+  <si>
+    <t>• Prover os resultados desejados pelos clientes, entregando software de qualidade
+• Trabalhar e ampliar conhecimentos de frontend e React.</t>
+  </si>
+  <si>
+    <t>• Prover os resultados desejados pelos clientes, entregando software de qualidade;
+• Trabalhar e ampliar conhecimentos de frontend e React.</t>
+  </si>
+  <si>
+    <t>• Prover os resultados desejados pelos clientes, entregando software de qualidade;
+• Maximizar a produtividade da equipe de desenvolvimento para que as entregas ocorram da melhor forma possível e dentro do prazo.</t>
+  </si>
+  <si>
+    <t>• Realizar reuniões frequentes a fim de compartilhar o que foi feito e quais as dificuldades encontradas;
+• Proporcionar recursos adequados para que o trabalho possa ser executado;
+• Fornecer feedbacks construtivos;
+• Reconhecer os esforços realizados;
+• Estimular o aprendizado constante e o trabalho em colaboração.</t>
+  </si>
+  <si>
+    <t>• Demonstrar respeito e confiança;
+• Realizar reuniões frequentes a fim de compartilhar o que foi feito e quais as dificuldades encontradas;
+• Proporcionar recursos adequados para que o trabalho possa ser executado;
+• Fornecer feedbacks construtivos;
+• Reconhecer os esforços realizados;
+• Estimular o aprendizado constante e o trabalho em colaboração.</t>
+  </si>
+  <si>
+    <t>• Homologar e validar requisitos;
+• Testar e utilizar a plataforma em sala de aula;
+ • Prover feedbacks detalhados de como a plataforma pode ser melhorada.</t>
+  </si>
+  <si>
+    <t>• Realizar entregas contínuas que agreguem valor ao cliente;
+• Manter o cliente informado sobre o estado do projeto;
+• Coletar os requisitos e os feedbacks do cliente para um melhor uso da plataforma em sala de aula.</t>
+  </si>
+  <si>
+    <t>• Fornecer estrutura física para realização do trabalho;
+• Proporcionar ambiente virtual institucional para implantação da plataforma;
+• Fomentar financeiramente o projeto.</t>
+  </si>
+  <si>
+    <t>Consumir um software acadêmico que possa ser aplicado no campus para permitir a aplicação e realização de atividades avaliativas por meio de um banco de questões</t>
+  </si>
+  <si>
+    <t>Prover os resultados desejados pelos clientes, entregando software de qualidade.</t>
+  </si>
+  <si>
+    <t>• Apresentar constantemente resultados que agregram valor;
+• Demonstrar esforço constante sob o software ofertado para a instituição, a fim de melhor atendê-la com qualidade e no menor tempo possível;
+• Se manter disponível para eventuais questionamentos e/ou reuniões;
+• Manter a instituição informada sobre o estado do projeto.</t>
+  </si>
+  <si>
+    <t>Órgão de fomento do projeto</t>
+  </si>
+  <si>
+    <t>Professor que utilizará o sistema produzido em sala de aula</t>
+  </si>
+  <si>
+    <t>Estudantes que utilizarão o sistema para realizar estudos</t>
+  </si>
+  <si>
+    <t>Usuário do sistema</t>
+  </si>
+  <si>
+    <t>Cliente e Usuário do sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+•  Dar exemplos de alunos que utilizaram o sistema e obtiveram um melhor desempenho acadêmico;
+• Demonstrar facilidade de uso da plataforma e fornecer treinamento sobre sua utilização se necessário;
+• Coletar feedbacks e sugestões.</t>
+  </si>
+  <si>
+    <t>Aluno - IFRN Campus Natal Central</t>
   </si>
 </sst>
 </file>
@@ -1296,19 +1343,6 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="44" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="36" borderId="0" xfId="44" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="44" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="12" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="44" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="44" applyFont="1" applyAlignment="1">
@@ -1317,6 +1351,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="36" borderId="0" xfId="44" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="44" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1332,6 +1369,16 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="58" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="44" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="44" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="12" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1986,13 +2033,13 @@
         <v>41</v>
       </c>
       <c r="E5" s="34"/>
-      <c r="F5" s="67" t="s">
+      <c r="F5" s="62" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="68"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
     </row>
     <row r="6" spans="1:10" s="30" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="31"/>
@@ -2032,90 +2079,90 @@
       <c r="B10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="72" t="s">
+      <c r="C10" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="72"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="68"/>
     </row>
     <row r="11" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="70" t="s">
+      <c r="C11" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="70"/>
-      <c r="E11" s="70"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="70" t="s">
+      <c r="D11" s="66"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="70"/>
-      <c r="I11" s="60" t="s">
+      <c r="H11" s="66"/>
+      <c r="I11" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="J11" s="60"/>
+      <c r="J11" s="70"/>
     </row>
     <row r="12" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="44">
         <v>1</v>
       </c>
-      <c r="C12" s="71" t="s">
+      <c r="C12" s="67" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="71"/>
-      <c r="E12" s="71"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="73" t="s">
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="H12" s="73"/>
-      <c r="I12" s="61"/>
-      <c r="J12" s="61"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="71"/>
+      <c r="J12" s="71"/>
     </row>
     <row r="13" spans="1:10" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="44">
         <f>B12+1</f>
         <v>2</v>
       </c>
-      <c r="C13" s="71" t="s">
+      <c r="C13" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="71"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="71"/>
-      <c r="G13" s="73" t="s">
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="73"/>
-      <c r="I13" s="61"/>
-      <c r="J13" s="61"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="71"/>
+      <c r="J13" s="71"/>
     </row>
     <row r="14" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="C14" s="69"/>
-      <c r="D14" s="69"/>
-      <c r="E14" s="69"/>
-      <c r="F14" s="69"/>
-      <c r="G14" s="64"/>
-      <c r="H14" s="64"/>
-      <c r="I14" s="62"/>
-      <c r="J14" s="62"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="73"/>
+      <c r="H14" s="73"/>
+      <c r="I14" s="72"/>
+      <c r="J14" s="72"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:10" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B16" s="63" t="s">
+      <c r="B16" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="63"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="63"/>
-      <c r="F16" s="63"/>
-      <c r="G16" s="63"/>
-      <c r="H16" s="63"/>
-      <c r="I16" s="63"/>
-      <c r="J16" s="63"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="64"/>
+      <c r="H16" s="64"/>
+      <c r="I16" s="64"/>
+      <c r="J16" s="64"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="40" t="s">
@@ -2127,50 +2174,50 @@
       <c r="D17" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="65" t="s">
+      <c r="E17" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="65"/>
-      <c r="G17" s="65"/>
-      <c r="H17" s="65"/>
-      <c r="I17" s="65"/>
-      <c r="J17" s="65"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="60"/>
+      <c r="J17" s="60"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="41"/>
       <c r="C18" s="41"/>
       <c r="D18" s="42"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="66"/>
-      <c r="H18" s="66"/>
-      <c r="I18" s="66"/>
-      <c r="J18" s="66"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="61"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="61"/>
+      <c r="J18" s="61"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="41"/>
       <c r="C19" s="41"/>
       <c r="D19" s="42"/>
-      <c r="E19" s="66"/>
-      <c r="F19" s="66"/>
-      <c r="G19" s="66"/>
-      <c r="H19" s="66"/>
-      <c r="I19" s="66"/>
-      <c r="J19" s="66"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="61"/>
+      <c r="J19" s="61"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="21" spans="2:10" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B21" s="63" t="s">
+      <c r="B21" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="63"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="63"/>
-      <c r="F21" s="63"/>
-      <c r="G21" s="63"/>
-      <c r="H21" s="63"/>
-      <c r="I21" s="63"/>
-      <c r="J21" s="63"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="64"/>
+      <c r="H21" s="64"/>
+      <c r="I21" s="64"/>
+      <c r="J21" s="64"/>
     </row>
     <row r="22" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="40" t="s">
@@ -2182,14 +2229,14 @@
       <c r="D22" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="65" t="s">
+      <c r="E22" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="F22" s="65"/>
-      <c r="G22" s="65"/>
-      <c r="H22" s="65"/>
-      <c r="I22" s="65"/>
-      <c r="J22" s="65"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="60"/>
+      <c r="I22" s="60"/>
+      <c r="J22" s="60"/>
     </row>
     <row r="23" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="41">
@@ -2197,12 +2244,12 @@
       </c>
       <c r="C23" s="41"/>
       <c r="D23" s="42"/>
-      <c r="E23" s="66"/>
-      <c r="F23" s="66"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="66"/>
-      <c r="I23" s="66"/>
-      <c r="J23" s="66"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="61"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="61"/>
+      <c r="I23" s="61"/>
+      <c r="J23" s="61"/>
     </row>
     <row r="24" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="41">
@@ -2210,12 +2257,12 @@
       </c>
       <c r="C24" s="41"/>
       <c r="D24" s="42"/>
-      <c r="E24" s="66"/>
-      <c r="F24" s="66"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="66"/>
-      <c r="I24" s="66"/>
-      <c r="J24" s="66"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="61"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="61"/>
+      <c r="J24" s="61"/>
     </row>
     <row r="25" spans="2:10" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="26" spans="2:10" ht="15.75" x14ac:dyDescent="0.25"/>
@@ -2243,6 +2290,12 @@
     <row r="48" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="B21:J21"/>
+    <mergeCell ref="G14:H14"/>
     <mergeCell ref="E22:J22"/>
     <mergeCell ref="E23:J23"/>
     <mergeCell ref="E24:J24"/>
@@ -2259,12 +2312,6 @@
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="B21:J21"/>
-    <mergeCell ref="G14:H14"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D5" location="PartesInteressadas!A1" display="Partes interessadas" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -2293,10 +2340,10 @@
   <dimension ref="B1:P29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="J9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2393,7 +2440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" ht="138" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="57">
         <v>1</v>
       </c>
@@ -2418,10 +2465,10 @@
         <v>75</v>
       </c>
       <c r="J4" s="57" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="K4" s="57" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="L4" s="52" t="s">
         <v>4</v>
@@ -2429,10 +2476,12 @@
       <c r="M4" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="57"/>
+      <c r="N4" s="57" t="s">
+        <v>94</v>
+      </c>
       <c r="O4" s="51"/>
     </row>
-    <row r="5" spans="2:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="57">
         <f>B4+1</f>
         <v>2</v>
@@ -2458,10 +2507,10 @@
         <v>75</v>
       </c>
       <c r="J5" s="57" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="K5" s="57" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="L5" s="52" t="s">
         <v>5</v>
@@ -2469,12 +2518,14 @@
       <c r="M5" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="N5" s="57"/>
+      <c r="N5" s="57" t="s">
+        <v>95</v>
+      </c>
       <c r="O5" s="57" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" s="20" customFormat="1" ht="123.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="57">
         <f t="shared" ref="B6:B29" si="1">B5+1</f>
         <v>3</v>
@@ -2500,10 +2551,10 @@
         <v>75</v>
       </c>
       <c r="J6" s="57" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="K6" s="57" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="L6" s="52" t="s">
         <v>4</v>
@@ -2511,10 +2562,12 @@
       <c r="M6" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="N6" s="57"/>
+      <c r="N6" s="57" t="s">
+        <v>94</v>
+      </c>
       <c r="O6" s="57"/>
     </row>
-    <row r="7" spans="2:16" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:16" s="20" customFormat="1" ht="132" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="57">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -2540,10 +2593,10 @@
         <v>75</v>
       </c>
       <c r="J7" s="57" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="K7" s="57" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="L7" s="52" t="s">
         <v>4</v>
@@ -2551,10 +2604,12 @@
       <c r="M7" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="N7" s="57"/>
+      <c r="N7" s="57" t="s">
+        <v>94</v>
+      </c>
       <c r="O7" s="57"/>
     </row>
-    <row r="8" spans="2:16" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:16" s="20" customFormat="1" ht="133.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="57">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -2570,7 +2625,7 @@
         <v>68</v>
       </c>
       <c r="F8" s="57" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="G8" s="59"/>
       <c r="H8" s="57" t="s">
@@ -2580,10 +2635,10 @@
         <v>75</v>
       </c>
       <c r="J8" s="57" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="K8" s="57" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="L8" s="52" t="s">
         <v>4</v>
@@ -2591,10 +2646,12 @@
       <c r="M8" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="N8" s="57"/>
+      <c r="N8" s="57" t="s">
+        <v>94</v>
+      </c>
       <c r="O8" s="57"/>
     </row>
-    <row r="9" spans="2:16" s="20" customFormat="1" ht="111.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:16" s="20" customFormat="1" ht="153" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="57">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -2604,10 +2661,10 @@
         <v>16</v>
       </c>
       <c r="D9" s="57" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E9" s="58" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F9" s="57"/>
       <c r="G9" s="57"/>
@@ -2615,13 +2672,13 @@
         <v>74</v>
       </c>
       <c r="I9" s="57" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="J9" s="57" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K9" s="57" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="L9" s="52" t="s">
         <v>6</v>
@@ -2630,13 +2687,13 @@
         <v>6</v>
       </c>
       <c r="N9" s="57" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="O9" s="57" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16" s="20" customFormat="1" ht="90" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" s="20" customFormat="1" ht="177" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="57">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -2646,24 +2703,24 @@
         <v>16</v>
       </c>
       <c r="D10" s="57" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E10" s="57"/>
       <c r="F10" s="57" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G10" s="57"/>
       <c r="H10" s="57" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I10" s="57" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="J10" s="57" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="K10" s="57" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="L10" s="52" t="s">
         <v>6</v>
@@ -2672,50 +2729,50 @@
         <v>6</v>
       </c>
       <c r="N10" s="57" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="O10" s="57" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="2:16" s="20" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" s="20" customFormat="1" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="57">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="C11" s="51">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D11" s="57" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="E11" s="57"/>
-      <c r="F11" s="57" t="s">
-        <v>82</v>
-      </c>
+      <c r="F11" s="57"/>
       <c r="G11" s="57"/>
       <c r="H11" s="57" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I11" s="57" t="s">
+        <v>105</v>
+      </c>
+      <c r="J11" s="57" t="s">
+        <v>86</v>
+      </c>
+      <c r="K11" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="J11" s="57" t="s">
-        <v>98</v>
-      </c>
-      <c r="K11" s="57" t="s">
-        <v>87</v>
-      </c>
       <c r="L11" s="52" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M11" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="N11" s="57"/>
+      <c r="N11" s="57" t="s">
+        <v>107</v>
+      </c>
       <c r="O11" s="57" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="2:16" s="20" customFormat="1" x14ac:dyDescent="0.2">
@@ -3609,7 +3666,7 @@
   <dimension ref="B2:F9"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>